<commit_message>
Upload reglog excel file
</commit_message>
<xml_diff>
--- a/assets/demonstracao-regressaologistica.xlsx
+++ b/assets/demonstracao-regressaologistica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\Desktop\ML_especializacao_2025\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9472692-3F4E-4DE3-8C9E-C8C71B46207C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8337503A-BF63-4A51-996E-57A410A2762B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5D7F5028-05B5-46F3-A4FA-FF6B84F5658A}"/>
+    <workbookView xWindow="3915" yWindow="225" windowWidth="15375" windowHeight="8895" xr2:uid="{5D7F5028-05B5-46F3-A4FA-FF6B84F5658A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>z</t>
   </si>
@@ -54,20 +54,6 @@
   </si>
   <si>
     <t>z = -8.79+1.37x</t>
-  </si>
-  <si>
-    <t>import numpy as np
-from sklearn.linear_model import LogisticRegression
-notas_simulados = [9, 7, 8, 3, 8, 7, 3, 8, 9, 7, 6, 5,7,5,2]
-notas_simulados = np.reshape(notas_simulados, (15,1))
-resultado = [1,1,1,0,1,1,0,1,1,0,0,0,1,0,0]
-resultado = np.reshape(resultado, (15,1))
-reglog = LogisticRegression(
-  random_state=0,
-  fit_intercept=True
-)
-reglog.fit(notas_simulados, resultado)
-reglog.__dict__</t>
   </si>
 </sst>
 </file>
@@ -122,7 +108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -145,77 +131,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -260,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,50 +192,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,7 +697,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -847,7 +735,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -1865,10 +1753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1294AA-43DE-4DCC-8B4C-6A0028EE8E7E}">
-  <dimension ref="A1:AC32"/>
+  <dimension ref="A1:AC17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1902,7 +1790,7 @@
         <v>-6.0499999999999989</v>
       </c>
       <c r="C2" s="8">
-        <f>1/(1+EXP(-B2))</f>
+        <f t="shared" ref="C2:C16" si="0">1/(1+EXP(-B2))</f>
         <v>2.35231557097815E-3</v>
       </c>
       <c r="D2" s="7" t="str">
@@ -1915,15 +1803,15 @@
         <v>3</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B16" si="0">-8.79+1.37*A3</f>
+        <f t="shared" ref="B3:B16" si="1">-8.79+1.37*A3</f>
         <v>-4.6799999999999988</v>
       </c>
       <c r="C3" s="8">
-        <f>1/(1+EXP(-B3))</f>
+        <f t="shared" si="0"/>
         <v>9.1937053672881026E-3</v>
       </c>
       <c r="D3" s="7" t="str">
-        <f t="shared" ref="D3:D16" si="1">IF(C3&gt;=0.75,"Aprovado","Reprovado")</f>
+        <f t="shared" ref="D3:D16" si="2">IF(C3&gt;=0.75,"Aprovado","Reprovado")</f>
         <v>Reprovado</v>
       </c>
     </row>
@@ -1932,15 +1820,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="7">
+        <f t="shared" si="1"/>
+        <v>-4.6799999999999988</v>
+      </c>
+      <c r="C4" s="8">
         <f t="shared" si="0"/>
-        <v>-4.6799999999999988</v>
-      </c>
-      <c r="C4" s="8">
-        <f>1/(1+EXP(-B4))</f>
         <v>9.1937053672881026E-3</v>
       </c>
       <c r="D4" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Reprovado</v>
       </c>
       <c r="O4" s="5"/>
@@ -1964,15 +1852,15 @@
         <v>5</v>
       </c>
       <c r="B5" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.9399999999999986</v>
+      </c>
+      <c r="C5" s="8">
         <f t="shared" si="0"/>
-        <v>-1.9399999999999986</v>
-      </c>
-      <c r="C5" s="8">
-        <f>1/(1+EXP(-B5))</f>
         <v>0.12564785651534582</v>
       </c>
       <c r="D5" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Reprovado</v>
       </c>
     </row>
@@ -1981,15 +1869,15 @@
         <v>5</v>
       </c>
       <c r="B6" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.9399999999999986</v>
+      </c>
+      <c r="C6" s="8">
         <f t="shared" si="0"/>
-        <v>-1.9399999999999986</v>
-      </c>
-      <c r="C6" s="8">
-        <f>1/(1+EXP(-B6))</f>
         <v>0.12564785651534582</v>
       </c>
       <c r="D6" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Reprovado</v>
       </c>
     </row>
@@ -1998,15 +1886,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.56999999999999851</v>
+      </c>
+      <c r="C7" s="8">
         <f t="shared" si="0"/>
-        <v>-0.56999999999999851</v>
-      </c>
-      <c r="C7" s="8">
-        <f>1/(1+EXP(-B7))</f>
         <v>0.36123682485115843</v>
       </c>
       <c r="D7" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Reprovado</v>
       </c>
     </row>
@@ -2015,15 +1903,15 @@
         <v>7</v>
       </c>
       <c r="B8" s="7">
+        <f t="shared" si="1"/>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="C8" s="8">
         <f t="shared" si="0"/>
-        <v>0.80000000000000071</v>
-      </c>
-      <c r="C8" s="8">
-        <f>1/(1+EXP(-B8))</f>
         <v>0.68997448112761262</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Reprovado</v>
       </c>
     </row>
@@ -2032,15 +1920,15 @@
         <v>7</v>
       </c>
       <c r="B9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="C9" s="8">
         <f t="shared" si="0"/>
-        <v>0.80000000000000071</v>
-      </c>
-      <c r="C9" s="8">
-        <f>1/(1+EXP(-B9))</f>
         <v>0.68997448112761262</v>
       </c>
       <c r="D9" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Reprovado</v>
       </c>
     </row>
@@ -2049,15 +1937,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="7">
+        <f t="shared" si="1"/>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="C10" s="8">
         <f t="shared" si="0"/>
-        <v>0.80000000000000071</v>
-      </c>
-      <c r="C10" s="8">
-        <f>1/(1+EXP(-B10))</f>
         <v>0.68997448112761262</v>
       </c>
       <c r="D10" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Reprovado</v>
       </c>
     </row>
@@ -2066,15 +1954,15 @@
         <v>7</v>
       </c>
       <c r="B11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="C11" s="8">
         <f t="shared" si="0"/>
-        <v>0.80000000000000071</v>
-      </c>
-      <c r="C11" s="8">
-        <f>1/(1+EXP(-B11))</f>
         <v>0.68997448112761262</v>
       </c>
       <c r="D11" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Reprovado</v>
       </c>
     </row>
@@ -2083,15 +1971,15 @@
         <v>8</v>
       </c>
       <c r="B12" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1700000000000017</v>
+      </c>
+      <c r="C12" s="8">
         <f t="shared" si="0"/>
-        <v>2.1700000000000017</v>
-      </c>
-      <c r="C12" s="8">
-        <f>1/(1+EXP(-B12))</f>
         <v>0.89752296655590269</v>
       </c>
       <c r="D12" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Aprovado</v>
       </c>
     </row>
@@ -2100,15 +1988,15 @@
         <v>8</v>
       </c>
       <c r="B13" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1700000000000017</v>
+      </c>
+      <c r="C13" s="8">
         <f t="shared" si="0"/>
-        <v>2.1700000000000017</v>
-      </c>
-      <c r="C13" s="8">
-        <f>1/(1+EXP(-B13))</f>
         <v>0.89752296655590269</v>
       </c>
       <c r="D13" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Aprovado</v>
       </c>
     </row>
@@ -2117,15 +2005,15 @@
         <v>8</v>
       </c>
       <c r="B14" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1700000000000017</v>
+      </c>
+      <c r="C14" s="8">
         <f t="shared" si="0"/>
-        <v>2.1700000000000017</v>
-      </c>
-      <c r="C14" s="8">
-        <f>1/(1+EXP(-B14))</f>
         <v>0.89752296655590269</v>
       </c>
       <c r="D14" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Aprovado</v>
       </c>
     </row>
@@ -2134,15 +2022,15 @@
         <v>9</v>
       </c>
       <c r="B15" s="7">
+        <f t="shared" si="1"/>
+        <v>3.5400000000000027</v>
+      </c>
+      <c r="C15" s="8">
         <f t="shared" si="0"/>
-        <v>3.5400000000000027</v>
-      </c>
-      <c r="C15" s="8">
-        <f>1/(1+EXP(-B15))</f>
         <v>0.97180471202985741</v>
       </c>
       <c r="D15" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Aprovado</v>
       </c>
     </row>
@@ -2151,15 +2039,15 @@
         <v>9</v>
       </c>
       <c r="B16" s="7">
+        <f t="shared" si="1"/>
+        <v>3.5400000000000027</v>
+      </c>
+      <c r="C16" s="8">
         <f t="shared" si="0"/>
-        <v>3.5400000000000027</v>
-      </c>
-      <c r="C16" s="8">
-        <f>1/(1+EXP(-B16))</f>
         <v>0.97180471202985741</v>
       </c>
       <c r="D16" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Aprovado</v>
       </c>
     </row>
@@ -2178,151 +2066,13 @@
       <c r="K17" s="10"/>
       <c r="L17" s="11"/>
     </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="14"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="17"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="17"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="17"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F22" s="15"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="17"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="17"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="17"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="17"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="17"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="17"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="17"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F29" s="15"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="17"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F30" s="15"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="17"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="17"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F32" s="18"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="20"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:D16" xr:uid="{0C1294AA-43DE-4DCC-8B4C-6A0028EE8E7E}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
       <sortCondition ref="A1:A16"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="F18:L32"/>
+  <mergeCells count="1">
     <mergeCell ref="F17:L17"/>
   </mergeCells>
   <conditionalFormatting sqref="D2:D16">

</xml_diff>

<commit_message>
Add blank sheet in logisticDemo
</commit_message>
<xml_diff>
--- a/assets/demonstracao-regressaologistica.xlsx
+++ b/assets/demonstracao-regressaologistica.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\Desktop\ML_especializacao_2025\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8337503A-BF63-4A51-996E-57A410A2762B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24FD062-75B1-48B6-A221-873BB4876B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="225" windowWidth="15375" windowHeight="8895" xr2:uid="{5D7F5028-05B5-46F3-A4FA-FF6B84F5658A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{5D7F5028-05B5-46F3-A4FA-FF6B84F5658A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="RegLog" sheetId="2" r:id="rId1"/>
+    <sheet name="blank" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$D$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">blank!$A$1:$D$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RegLog!$A$1:$D$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>z</t>
   </si>
@@ -214,7 +216,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -332,7 +344,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$C$1</c:f>
+              <c:f>RegLog!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -422,7 +434,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$16</c:f>
+              <c:f>RegLog!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="15"/>
@@ -476,7 +488,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Planilha1!$C$2:$C$16</c:f>
+              <c:f>RegLog!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -525,6 +537,562 @@
                 <c:pt idx="14">
                   <c:v>0.97180471202985741</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-98F3-4A7C-A396-14FD8D16C195}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1655926063"/>
+        <c:axId val="1655910703"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1655926063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Nota</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> Simulado</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1655910703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1655910703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" b="0" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>P(Y=1)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1655926063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Função sigmoide</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18393349268841394"/>
+          <c:y val="0.16622972120774102"/>
+          <c:w val="0.75042932133483309"/>
+          <c:h val="0.63512236884313622"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>blank!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>f(z)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>blank!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>blank!$C$2:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -879,6 +1447,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1395,7 +2003,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C92B847-5D9D-4936-876A-C110C226FD12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1752,11 +2919,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1294AA-43DE-4DCC-8B4C-6A0028EE8E7E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D5ABB3-33DA-4ACD-B787-741417659DDF}">
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,12 +2957,12 @@
         <v>-6.0499999999999989</v>
       </c>
       <c r="C2" s="8">
-        <f t="shared" ref="C2:C16" si="0">1/(1+EXP(-B2))</f>
+        <f>1/(1+EXP(-B2))</f>
         <v>2.35231557097815E-3</v>
       </c>
-      <c r="D2" s="7" t="str">
-        <f>IF(C2&gt;=0.75,"Aprovado","Reprovado")</f>
-        <v>Reprovado</v>
+      <c r="D2" s="7">
+        <f>IF(C2&gt;=0.6,1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -1803,16 +2970,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B16" si="1">-8.79+1.37*A3</f>
+        <f>-8.79+1.37*A3</f>
         <v>-4.6799999999999988</v>
       </c>
       <c r="C3" s="8">
-        <f t="shared" si="0"/>
+        <f>1/(1+EXP(-B3))</f>
         <v>9.1937053672881026E-3</v>
       </c>
-      <c r="D3" s="7" t="str">
-        <f t="shared" ref="D3:D16" si="2">IF(C3&gt;=0.75,"Aprovado","Reprovado")</f>
-        <v>Reprovado</v>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D16" si="0">IF(C3&gt;=0.6,1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -1820,16 +2987,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B4:B16" si="1">-8.79+1.37*A4</f>
         <v>-4.6799999999999988</v>
       </c>
       <c r="C4" s="8">
+        <f t="shared" ref="C4:C16" si="2">1/(1+EXP(-B4))</f>
+        <v>9.1937053672881026E-3</v>
+      </c>
+      <c r="D4" s="7">
         <f t="shared" si="0"/>
-        <v>9.1937053672881026E-3</v>
-      </c>
-      <c r="D4" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Reprovado</v>
+        <v>0</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
@@ -1856,12 +3023,12 @@
         <v>-1.9399999999999986</v>
       </c>
       <c r="C5" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12564785651534582</v>
+      </c>
+      <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>0.12564785651534582</v>
-      </c>
-      <c r="D5" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Reprovado</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -1873,12 +3040,12 @@
         <v>-1.9399999999999986</v>
       </c>
       <c r="C6" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12564785651534582</v>
+      </c>
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>0.12564785651534582</v>
-      </c>
-      <c r="D6" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Reprovado</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -1890,12 +3057,12 @@
         <v>-0.56999999999999851</v>
       </c>
       <c r="C7" s="8">
+        <f t="shared" si="2"/>
+        <v>0.36123682485115843</v>
+      </c>
+      <c r="D7" s="7">
         <f t="shared" si="0"/>
-        <v>0.36123682485115843</v>
-      </c>
-      <c r="D7" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Reprovado</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -1907,12 +3074,12 @@
         <v>0.80000000000000071</v>
       </c>
       <c r="C8" s="8">
+        <f t="shared" si="2"/>
+        <v>0.68997448112761262</v>
+      </c>
+      <c r="D8" s="7">
         <f t="shared" si="0"/>
-        <v>0.68997448112761262</v>
-      </c>
-      <c r="D8" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Reprovado</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
@@ -1924,12 +3091,12 @@
         <v>0.80000000000000071</v>
       </c>
       <c r="C9" s="8">
+        <f t="shared" si="2"/>
+        <v>0.68997448112761262</v>
+      </c>
+      <c r="D9" s="7">
         <f t="shared" si="0"/>
-        <v>0.68997448112761262</v>
-      </c>
-      <c r="D9" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Reprovado</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
@@ -1941,12 +3108,12 @@
         <v>0.80000000000000071</v>
       </c>
       <c r="C10" s="8">
+        <f t="shared" si="2"/>
+        <v>0.68997448112761262</v>
+      </c>
+      <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>0.68997448112761262</v>
-      </c>
-      <c r="D10" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Reprovado</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -1958,12 +3125,12 @@
         <v>0.80000000000000071</v>
       </c>
       <c r="C11" s="8">
+        <f t="shared" si="2"/>
+        <v>0.68997448112761262</v>
+      </c>
+      <c r="D11" s="7">
         <f t="shared" si="0"/>
-        <v>0.68997448112761262</v>
-      </c>
-      <c r="D11" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Reprovado</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
@@ -1975,12 +3142,12 @@
         <v>2.1700000000000017</v>
       </c>
       <c r="C12" s="8">
+        <f t="shared" si="2"/>
+        <v>0.89752296655590269</v>
+      </c>
+      <c r="D12" s="7">
         <f t="shared" si="0"/>
-        <v>0.89752296655590269</v>
-      </c>
-      <c r="D12" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Aprovado</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
@@ -1992,12 +3159,12 @@
         <v>2.1700000000000017</v>
       </c>
       <c r="C13" s="8">
+        <f t="shared" si="2"/>
+        <v>0.89752296655590269</v>
+      </c>
+      <c r="D13" s="7">
         <f t="shared" si="0"/>
-        <v>0.89752296655590269</v>
-      </c>
-      <c r="D13" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Aprovado</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -2009,12 +3176,12 @@
         <v>2.1700000000000017</v>
       </c>
       <c r="C14" s="8">
+        <f t="shared" si="2"/>
+        <v>0.89752296655590269</v>
+      </c>
+      <c r="D14" s="7">
         <f t="shared" si="0"/>
-        <v>0.89752296655590269</v>
-      </c>
-      <c r="D14" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Aprovado</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
@@ -2026,12 +3193,12 @@
         <v>3.5400000000000027</v>
       </c>
       <c r="C15" s="8">
+        <f t="shared" si="2"/>
+        <v>0.97180471202985741</v>
+      </c>
+      <c r="D15" s="7">
         <f t="shared" si="0"/>
-        <v>0.97180471202985741</v>
-      </c>
-      <c r="D15" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Aprovado</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -2043,12 +3210,12 @@
         <v>3.5400000000000027</v>
       </c>
       <c r="C16" s="8">
+        <f t="shared" si="2"/>
+        <v>0.97180471202985741</v>
+      </c>
+      <c r="D16" s="7">
         <f t="shared" si="0"/>
-        <v>0.97180471202985741</v>
-      </c>
-      <c r="D16" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Aprovado</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2083,4 +3250,203 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1294AA-43DE-4DCC-8B4C-6A0028EE8E7E}">
+  <dimension ref="A1:AC17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>3</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>5</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>7</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="F17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D16" xr:uid="{0C1294AA-43DE-4DCC-8B4C-6A0028EE8E7E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D16">
+      <sortCondition ref="B1:B16"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="F17:L17"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D2:D16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Aprovado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>